<commit_message>
Atualização código grade curricular + excel
código em python atualizado + planilha excel excluido as 3 ultimas linhas
</commit_message>
<xml_diff>
--- a/grade_curricular.xlsx
+++ b/grade_curricular.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Convidado\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymundo\Documentos\Estudos\UFPR-Estatistica\2_Periodo\CE303 - Visualização de Dados Aplicada\Seminario\visual_grade_curricular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB90E8E6-8F39-4743-A686-596941DFE843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0220ED85-4207-4FF5-8F75-5F00C556F040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1695F74A-3941-4A80-A11F-AD4164E96C5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1695F74A-3941-4A80-A11F-AD4164E96C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$93</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="345">
   <si>
     <t>Período</t>
   </si>
@@ -493,15 +493,6 @@
   </si>
   <si>
     <t>Optativas</t>
-  </si>
-  <si>
-    <t>ACE I</t>
-  </si>
-  <si>
-    <t>ACE II</t>
-  </si>
-  <si>
-    <t>Projeto de Análise de Dados</t>
   </si>
   <si>
     <t>Processos Estocasticos</t>
@@ -1600,24 +1591,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891BC5F-22CD-4866-B0DC-0723F8DA3CD8}">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="45.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" style="3" customWidth="1"/>
     <col min="7" max="7" width="32" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1634,13 +1625,13 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1654,13 +1645,13 @@
         <v>60</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1674,13 +1665,13 @@
         <v>120</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -1694,13 +1685,13 @@
         <v>60</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1714,13 +1705,13 @@
         <v>60</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1737,13 +1728,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1760,13 +1751,13 @@
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1780,13 +1771,13 @@
         <v>60</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1800,13 +1791,13 @@
         <v>60</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1823,13 +1814,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1846,13 +1837,13 @@
         <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1869,13 +1860,13 @@
         <v>5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1889,13 +1880,13 @@
         <v>60</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1912,13 +1903,13 @@
         <v>6</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1935,13 +1926,13 @@
         <v>21</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1958,13 +1949,13 @@
         <v>43</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1981,13 +1972,13 @@
         <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2004,13 +1995,13 @@
         <v>44</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -2027,13 +2018,13 @@
         <v>39</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -2050,13 +2041,13 @@
         <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -2073,13 +2064,13 @@
         <v>56</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2096,13 +2087,13 @@
         <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -2119,13 +2110,13 @@
         <v>5</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
@@ -2142,13 +2133,13 @@
         <v>45</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -2165,13 +2156,13 @@
         <v>63</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -2188,13 +2179,13 @@
         <v>64</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2211,13 +2202,13 @@
         <v>65</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
@@ -2234,13 +2225,13 @@
         <v>45</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>79</v>
       </c>
@@ -2257,13 +2248,13 @@
         <v>77</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
@@ -2280,13 +2271,13 @@
         <v>77</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -2303,13 +2294,13 @@
         <v>78</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
@@ -2326,13 +2317,13 @@
         <v>71</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
@@ -2349,13 +2340,13 @@
         <v>85</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>154</v>
       </c>
@@ -2369,13 +2360,13 @@
         <v>60</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>154</v>
       </c>
@@ -2389,13 +2380,13 @@
         <v>60</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>154</v>
       </c>
@@ -2409,13 +2400,13 @@
         <v>60</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>154</v>
       </c>
@@ -2423,19 +2414,19 @@
         <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D37" s="1">
         <v>60</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>154</v>
       </c>
@@ -2449,13 +2440,13 @@
         <v>60</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>154</v>
       </c>
@@ -2469,13 +2460,13 @@
         <v>60</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>154</v>
       </c>
@@ -2489,13 +2480,13 @@
         <v>60</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>154</v>
       </c>
@@ -2509,13 +2500,13 @@
         <v>60</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>154</v>
       </c>
@@ -2529,13 +2520,13 @@
         <v>60</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>154</v>
       </c>
@@ -2549,13 +2540,13 @@
         <v>60</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>154</v>
       </c>
@@ -2569,13 +2560,13 @@
         <v>60</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>154</v>
       </c>
@@ -2589,13 +2580,13 @@
         <v>60</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>154</v>
       </c>
@@ -2609,13 +2600,13 @@
         <v>60</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>154</v>
       </c>
@@ -2629,13 +2620,13 @@
         <v>60</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>154</v>
       </c>
@@ -2649,13 +2640,13 @@
         <v>60</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>154</v>
       </c>
@@ -2669,13 +2660,13 @@
         <v>60</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>154</v>
       </c>
@@ -2689,13 +2680,13 @@
         <v>60</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>154</v>
       </c>
@@ -2703,19 +2694,19 @@
         <v>86</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D51" s="1">
         <v>60</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>154</v>
       </c>
@@ -2723,19 +2714,19 @@
         <v>87</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D52" s="1">
         <v>60</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>154</v>
       </c>
@@ -2743,19 +2734,19 @@
         <v>88</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D53" s="1">
         <v>60</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>154</v>
       </c>
@@ -2763,19 +2754,19 @@
         <v>89</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D54" s="1">
         <v>60</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>154</v>
       </c>
@@ -2783,19 +2774,19 @@
         <v>90</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D55" s="1">
         <v>60</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>154</v>
       </c>
@@ -2803,19 +2794,19 @@
         <v>91</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D56" s="1">
         <v>60</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>154</v>
       </c>
@@ -2823,19 +2814,19 @@
         <v>92</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D57" s="1">
         <v>60</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>154</v>
       </c>
@@ -2843,19 +2834,19 @@
         <v>93</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D58" s="1">
         <v>60</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>154</v>
       </c>
@@ -2863,19 +2854,19 @@
         <v>94</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D59" s="1">
         <v>60</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>154</v>
       </c>
@@ -2883,19 +2874,19 @@
         <v>95</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D60" s="1">
         <v>60</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>154</v>
       </c>
@@ -2903,19 +2894,19 @@
         <v>96</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D61" s="1">
         <v>60</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>154</v>
       </c>
@@ -2923,19 +2914,19 @@
         <v>97</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D62" s="1">
         <v>60</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>154</v>
       </c>
@@ -2943,19 +2934,19 @@
         <v>98</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D63" s="1">
         <v>60</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>154</v>
       </c>
@@ -2963,19 +2954,19 @@
         <v>99</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D64" s="1">
         <v>60</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>154</v>
       </c>
@@ -2983,19 +2974,19 @@
         <v>100</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D65" s="1">
         <v>60</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>154</v>
       </c>
@@ -3003,19 +2994,19 @@
         <v>101</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D66" s="1">
         <v>60</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>154</v>
       </c>
@@ -3023,19 +3014,19 @@
         <v>102</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D67" s="1">
         <v>60</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>154</v>
       </c>
@@ -3043,19 +3034,19 @@
         <v>103</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D68" s="1">
         <v>60</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>154</v>
       </c>
@@ -3063,19 +3054,19 @@
         <v>104</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D69" s="1">
         <v>60</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>154</v>
       </c>
@@ -3083,19 +3074,19 @@
         <v>105</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D70" s="1">
         <v>60</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -3103,19 +3094,19 @@
         <v>106</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D71" s="1">
         <v>60</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>154</v>
       </c>
@@ -3123,19 +3114,19 @@
         <v>107</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D72" s="1">
         <v>60</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>154</v>
       </c>
@@ -3143,19 +3134,19 @@
         <v>108</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D73" s="1">
         <v>30</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>154</v>
       </c>
@@ -3163,19 +3154,19 @@
         <v>109</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D74" s="1">
         <v>60</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>154</v>
       </c>
@@ -3183,19 +3174,19 @@
         <v>110</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D75" s="1">
         <v>60</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>154</v>
       </c>
@@ -3203,19 +3194,19 @@
         <v>111</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D76" s="1">
         <v>60</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>154</v>
       </c>
@@ -3223,19 +3214,19 @@
         <v>112</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D77" s="1">
         <v>60</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>154</v>
       </c>
@@ -3243,19 +3234,19 @@
         <v>113</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D78" s="1">
         <v>60</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>154</v>
       </c>
@@ -3263,19 +3254,19 @@
         <v>114</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D79" s="1">
         <v>60</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>154</v>
       </c>
@@ -3283,19 +3274,19 @@
         <v>115</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D80" s="1">
         <v>60</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>154</v>
       </c>
@@ -3303,19 +3294,19 @@
         <v>116</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D81" s="1">
         <v>60</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>154</v>
       </c>
@@ -3323,19 +3314,19 @@
         <v>117</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D82" s="1">
         <v>60</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>154</v>
       </c>
@@ -3343,19 +3334,19 @@
         <v>118</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D83" s="1">
         <v>60</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>154</v>
       </c>
@@ -3363,19 +3354,19 @@
         <v>119</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D84" s="1">
         <v>60</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>154</v>
       </c>
@@ -3383,19 +3374,19 @@
         <v>120</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D85" s="1">
         <v>60</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>154</v>
       </c>
@@ -3403,19 +3394,19 @@
         <v>121</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D86" s="1">
         <v>60</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>154</v>
       </c>
@@ -3423,19 +3414,19 @@
         <v>122</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D87" s="1">
         <v>60</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>154</v>
       </c>
@@ -3443,19 +3434,19 @@
         <v>123</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D88" s="1">
         <v>60</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>154</v>
       </c>
@@ -3463,19 +3454,19 @@
         <v>124</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D89" s="1">
         <v>60</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>154</v>
       </c>
@@ -3483,19 +3474,19 @@
         <v>125</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D90" s="1">
         <v>60</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>154</v>
       </c>
@@ -3503,19 +3494,19 @@
         <v>126</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D91" s="1">
         <v>60</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>154</v>
       </c>
@@ -3523,19 +3514,19 @@
         <v>127</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D92" s="1">
         <v>60</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>154</v>
       </c>
@@ -3543,68 +3534,20 @@
         <v>128</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D93" s="1">
         <v>60</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D94" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D95" s="1">
-        <v>240</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C96" t="s">
-        <v>157</v>
-      </c>
-      <c r="D96" s="1">
-        <v>180</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>43</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G96" xr:uid="{C891BC5F-22CD-4866-B0DC-0723F8DA3CD8}"/>
+  <autoFilter ref="A1:G93" xr:uid="{C891BC5F-22CD-4866-B0DC-0723F8DA3CD8}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>